<commit_message>
start handling of metadata.
</commit_message>
<xml_diff>
--- a/dataset_sample_2rows.xlsx
+++ b/dataset_sample_2rows.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ot2661/Documents/01_dev/aed_pub/regimo/regimo/services/backend_regimo/data/LLEC_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF64A3FC-614A-BE47-BE9C-852C763A5AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCD2905-E186-AF44-8861-1775FA62A05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="500" windowWidth="19800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4980" yWindow="5900" windowWidth="30520" windowHeight="15980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_sample_2rows_comp" sheetId="1" r:id="rId1"/>
+    <sheet name="dataset_sample_2rows_meta" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="240">
   <si>
     <t>t_amb</t>
   </si>
@@ -354,14 +355,432 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>Ambient temperature</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>temperture</t>
+  </si>
+  <si>
+    <t>http://openenergy-platform.org/ontology/oeo/OEO_00010453</t>
+  </si>
+  <si>
+    <t>[°C]</t>
+  </si>
+  <si>
+    <t>Solar radiation</t>
+  </si>
+  <si>
+    <t>solar radiation</t>
+  </si>
+  <si>
+    <t>https://openenergyplatform.org/ontology/oeo/OEO_00020038/</t>
+  </si>
+  <si>
+    <t>[W/m²]</t>
+  </si>
+  <si>
+    <t>Relative humidity</t>
+  </si>
+  <si>
+    <t>relative humidity</t>
+  </si>
+  <si>
+    <t>[%]</t>
+  </si>
+  <si>
+    <t>Wind velocity</t>
+  </si>
+  <si>
+    <t>wind velocity</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000060</t>
+  </si>
+  <si>
+    <t>[m/s]</t>
+  </si>
+  <si>
+    <t>Heat pump's secondary loop thermal power</t>
+  </si>
+  <si>
+    <t>power unit</t>
+  </si>
+  <si>
+    <t>https://openenergyplatform.org/ontology/oeo/OEO_00000333/</t>
+  </si>
+  <si>
+    <t>[W]</t>
+  </si>
+  <si>
+    <t>Heat pump's primary loop thermal power</t>
+  </si>
+  <si>
+    <t>Heat pump's secondary loop supply temperature</t>
+  </si>
+  <si>
+    <t>Heat pump's secondary loop return temperature</t>
+  </si>
+  <si>
+    <t>Heat pump's secondary loop volume flow rate</t>
+  </si>
+  <si>
+    <t>water flow rate</t>
+  </si>
+  <si>
+    <t>https://openenergyplatform.org/ontology/oeo/OEO_00110003/</t>
+  </si>
+  <si>
+    <t>[m³/h]</t>
+  </si>
+  <si>
+    <t>Heat pump's primary loop supply temperature</t>
+  </si>
+  <si>
+    <t>Heat pump's primary loop return temperature</t>
+  </si>
+  <si>
+    <t>Heat pump's primary loop volume flow rate</t>
+  </si>
+  <si>
+    <t>Brine flow rate</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000270</t>
+  </si>
+  <si>
+    <t>Delivered heat to room 1</t>
+  </si>
+  <si>
+    <t>Delivered heat to room 2</t>
+  </si>
+  <si>
+    <t>Delivered heat to room 3</t>
+  </si>
+  <si>
+    <t>Delivered heat to room 4 by its first circuit</t>
+  </si>
+  <si>
+    <t>Delivered heat to room 4 by its second circuit</t>
+  </si>
+  <si>
+    <t>Delivered heat to room 5 by its first circuit</t>
+  </si>
+  <si>
+    <t>Delivered heat to room 5 by its second circuit</t>
+  </si>
+  <si>
+    <t>Delivered heat to bathroom</t>
+  </si>
+  <si>
+    <t>Delivered heat to kitchen</t>
+  </si>
+  <si>
+    <t>Delivered heat to corridor</t>
+  </si>
+  <si>
+    <t>Supply temperature of room 1</t>
+  </si>
+  <si>
+    <t>Return temperature of room 1</t>
+  </si>
+  <si>
+    <t>Volume flow rate of room 1's heating circuit</t>
+  </si>
+  <si>
+    <t>Supply temperature of room 2</t>
+  </si>
+  <si>
+    <t>Return temperature of room 2</t>
+  </si>
+  <si>
+    <t>Volume flow rate of room 2's heating circuit</t>
+  </si>
+  <si>
+    <t>Supply temperature of room 3</t>
+  </si>
+  <si>
+    <t>Return temperature of room 3</t>
+  </si>
+  <si>
+    <t>Volume flow rate of room 3's heating circuit</t>
+  </si>
+  <si>
+    <t>Supply temperature of room 4's first heating circuit</t>
+  </si>
+  <si>
+    <t>Return temperature of room 4's first heating circuit</t>
+  </si>
+  <si>
+    <t>Volume flow rate of room 4's first heating circuit</t>
+  </si>
+  <si>
+    <t>Supply temperature of room 4's second heating circuit</t>
+  </si>
+  <si>
+    <t>Return temperature of room 4's second heating circuit</t>
+  </si>
+  <si>
+    <t>Volume flow rate of room 4's second heating circuit</t>
+  </si>
+  <si>
+    <t>Supply temperature of room 5's first heating circuit</t>
+  </si>
+  <si>
+    <t>Return temperature of room 5's first heating circuit</t>
+  </si>
+  <si>
+    <t>Volume flow rate of room 5's first heating circuit</t>
+  </si>
+  <si>
+    <t>Supply temperature of room 5's second heating circuit</t>
+  </si>
+  <si>
+    <t>Return temperature of room 5's second heating circuit</t>
+  </si>
+  <si>
+    <t>Volume flow rate of room 5's second heating circuit</t>
+  </si>
+  <si>
+    <t>Suppy temperature of bathroom</t>
+  </si>
+  <si>
+    <t>Return temperature of bathroom</t>
+  </si>
+  <si>
+    <t>Volume flow rate of bathroom's heating circuit</t>
+  </si>
+  <si>
+    <t>Suppy temperature of kitchen</t>
+  </si>
+  <si>
+    <t>Return temperature of kitchen</t>
+  </si>
+  <si>
+    <t>Volume flow rate of kitchen's heating circuit</t>
+  </si>
+  <si>
+    <t>Suppy temperature of corridor</t>
+  </si>
+  <si>
+    <t>Return temperature of corridor</t>
+  </si>
+  <si>
+    <t>Volume flow rate of corridor's heating circuit</t>
+  </si>
+  <si>
+    <t>Room 1 temperature</t>
+  </si>
+  <si>
+    <t>Room 1 setpoint temperature</t>
+  </si>
+  <si>
+    <t>Room 2 temperature</t>
+  </si>
+  <si>
+    <t>Room 2 setpoint temperature</t>
+  </si>
+  <si>
+    <t>Room 3 temperature</t>
+  </si>
+  <si>
+    <t>Room 3 setpoint temperature</t>
+  </si>
+  <si>
+    <t>Room 4 temperature</t>
+  </si>
+  <si>
+    <t>Room 4 setpoint temperature</t>
+  </si>
+  <si>
+    <t>Room 5 temperature</t>
+  </si>
+  <si>
+    <t>Room 5 setpoint temperature</t>
+  </si>
+  <si>
+    <t>Bath temperature</t>
+  </si>
+  <si>
+    <t>Bath setpoint temperature</t>
+  </si>
+  <si>
+    <t>Kitchen temperature</t>
+  </si>
+  <si>
+    <t>Kitchen setpoint temperature</t>
+  </si>
+  <si>
+    <t>Corridor temperature</t>
+  </si>
+  <si>
+    <t>Corridor setpoint temperature</t>
+  </si>
+  <si>
+    <t>U-probe 1 temperature at 1m depth</t>
+  </si>
+  <si>
+    <t>U-probe 1 temperature at 5m depth</t>
+  </si>
+  <si>
+    <t>U-probe 1 temperature at 10m depth</t>
+  </si>
+  <si>
+    <t>U-probe 1 temperature at 18m depth</t>
+  </si>
+  <si>
+    <t>U-probe 1 temperature at 27m depth</t>
+  </si>
+  <si>
+    <t>U-probe 1 temperature at 37m depth</t>
+  </si>
+  <si>
+    <t>U-probe 2 temperature at 1m depth</t>
+  </si>
+  <si>
+    <t>U-probe 2 temperature at 5m depth</t>
+  </si>
+  <si>
+    <t>U-probe 2 temperature at 10m depth</t>
+  </si>
+  <si>
+    <t>U-probe 2 temperature at 18m depth</t>
+  </si>
+  <si>
+    <t>U-probe 2 temperature at 27m depth</t>
+  </si>
+  <si>
+    <t>U-probe 2 temperature at 37m depth</t>
+  </si>
+  <si>
+    <t>U-probe 3 temperature at 1m depth</t>
+  </si>
+  <si>
+    <t>U-probe 3 temperature at 5m depth</t>
+  </si>
+  <si>
+    <t>U-probe 3 temperature at 10m depth</t>
+  </si>
+  <si>
+    <t>U-probe 3 temperature at 18m depth</t>
+  </si>
+  <si>
+    <t>U-probe 3 temperature at 27m depth</t>
+  </si>
+  <si>
+    <t>Water level monitor 1 temperature at 1m depth</t>
+  </si>
+  <si>
+    <t>Water level monitor 1 temperature at 5m depth</t>
+  </si>
+  <si>
+    <t>Water level monitor 1 temperature at 10m depth</t>
+  </si>
+  <si>
+    <t>Water level monitor 2 temperature at 1m depth</t>
+  </si>
+  <si>
+    <t>Water level monitor 2 temperature at 5m depth</t>
+  </si>
+  <si>
+    <t>Water level monitor 2 temperature at 10m depth</t>
+  </si>
+  <si>
+    <t>Water level monitor 3 temperature at 1m depth</t>
+  </si>
+  <si>
+    <t>Water level monitor 3 temperature at 5m depth</t>
+  </si>
+  <si>
+    <t>Water level monitor 3 temperature at 10m depth</t>
+  </si>
+  <si>
+    <t>Spiral probe temperature at 1m depth</t>
+  </si>
+  <si>
+    <t>Spiral probe temperature at 10m depth</t>
+  </si>
+  <si>
+    <t>Spiral probe temperature at 18m depth</t>
+  </si>
+  <si>
+    <t>Water level monitor 4 temperature at 1m depth</t>
+  </si>
+  <si>
+    <t>Water level monitor 4 temperature at 5m depth</t>
+  </si>
+  <si>
+    <t>Water level monitor 4 temperature at 10m depth</t>
+  </si>
+  <si>
+    <t>Water level monitor 4 temperature at 18m depth</t>
+  </si>
+  <si>
+    <t>Power at grid connection point</t>
+  </si>
+  <si>
+    <t>Photovoltaic generated power</t>
+  </si>
+  <si>
+    <t>Power consumption of heat pump</t>
+  </si>
+  <si>
+    <t>Power consumption of kitchen appliances</t>
+  </si>
+  <si>
+    <t>isAbout.name</t>
+  </si>
+  <si>
+    <t>isAbout.path</t>
+  </si>
+  <si>
+    <t>valueReference.value</t>
+  </si>
+  <si>
+    <t>valueReference.name</t>
+  </si>
+  <si>
+    <t>valueReference.path</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -386,15 +805,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -675,7 +1102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1579,4 +2006,3113 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D989DE-C4AF-CF4B-A769-6611C82EBD6C}">
+  <dimension ref="A1:I106"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="I5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H6" t="s">
+        <v>128</v>
+      </c>
+      <c r="I6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" t="s">
+        <v>128</v>
+      </c>
+      <c r="I7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F10" t="s">
+        <v>134</v>
+      </c>
+      <c r="G10" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10" t="s">
+        <v>135</v>
+      </c>
+      <c r="I10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" t="s">
+        <v>112</v>
+      </c>
+      <c r="G11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H11" t="s">
+        <v>113</v>
+      </c>
+      <c r="I11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" t="s">
+        <v>112</v>
+      </c>
+      <c r="H12" t="s">
+        <v>113</v>
+      </c>
+      <c r="I12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F13" t="s">
+        <v>140</v>
+      </c>
+      <c r="G13" t="s">
+        <v>140</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" t="s">
+        <v>127</v>
+      </c>
+      <c r="G14" t="s">
+        <v>127</v>
+      </c>
+      <c r="H14" t="s">
+        <v>128</v>
+      </c>
+      <c r="I14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" t="s">
+        <v>127</v>
+      </c>
+      <c r="G15" t="s">
+        <v>127</v>
+      </c>
+      <c r="H15" t="s">
+        <v>128</v>
+      </c>
+      <c r="I15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H16" t="s">
+        <v>128</v>
+      </c>
+      <c r="I16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" t="s">
+        <v>127</v>
+      </c>
+      <c r="H17" t="s">
+        <v>128</v>
+      </c>
+      <c r="I17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G18" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" t="s">
+        <v>127</v>
+      </c>
+      <c r="E19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" t="s">
+        <v>127</v>
+      </c>
+      <c r="G19" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" t="s">
+        <v>128</v>
+      </c>
+      <c r="I19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F20" t="s">
+        <v>127</v>
+      </c>
+      <c r="G20" t="s">
+        <v>127</v>
+      </c>
+      <c r="H20" t="s">
+        <v>128</v>
+      </c>
+      <c r="I20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G21" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" t="s">
+        <v>128</v>
+      </c>
+      <c r="I21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" t="s">
+        <v>127</v>
+      </c>
+      <c r="E22" t="s">
+        <v>128</v>
+      </c>
+      <c r="F22" t="s">
+        <v>127</v>
+      </c>
+      <c r="G22" t="s">
+        <v>127</v>
+      </c>
+      <c r="H22" t="s">
+        <v>128</v>
+      </c>
+      <c r="I22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" t="s">
+        <v>128</v>
+      </c>
+      <c r="F23" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" t="s">
+        <v>127</v>
+      </c>
+      <c r="H23" t="s">
+        <v>128</v>
+      </c>
+      <c r="I23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" t="s">
+        <v>112</v>
+      </c>
+      <c r="H24" t="s">
+        <v>113</v>
+      </c>
+      <c r="I24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" t="s">
+        <v>113</v>
+      </c>
+      <c r="I25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E26" t="s">
+        <v>135</v>
+      </c>
+      <c r="F26" t="s">
+        <v>134</v>
+      </c>
+      <c r="G26" t="s">
+        <v>134</v>
+      </c>
+      <c r="H26" t="s">
+        <v>135</v>
+      </c>
+      <c r="I26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27" t="s">
+        <v>112</v>
+      </c>
+      <c r="H27" t="s">
+        <v>113</v>
+      </c>
+      <c r="I27" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G28" t="s">
+        <v>112</v>
+      </c>
+      <c r="H28" t="s">
+        <v>113</v>
+      </c>
+      <c r="I28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" t="s">
+        <v>134</v>
+      </c>
+      <c r="E29" t="s">
+        <v>135</v>
+      </c>
+      <c r="F29" t="s">
+        <v>134</v>
+      </c>
+      <c r="G29" t="s">
+        <v>134</v>
+      </c>
+      <c r="H29" t="s">
+        <v>135</v>
+      </c>
+      <c r="I29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>158</v>
+      </c>
+      <c r="C30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" t="s">
+        <v>113</v>
+      </c>
+      <c r="F30" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" t="s">
+        <v>112</v>
+      </c>
+      <c r="H30" t="s">
+        <v>113</v>
+      </c>
+      <c r="I30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>159</v>
+      </c>
+      <c r="C31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" t="s">
+        <v>112</v>
+      </c>
+      <c r="G31" t="s">
+        <v>112</v>
+      </c>
+      <c r="H31" t="s">
+        <v>113</v>
+      </c>
+      <c r="I31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" t="s">
+        <v>134</v>
+      </c>
+      <c r="E32" t="s">
+        <v>135</v>
+      </c>
+      <c r="F32" t="s">
+        <v>134</v>
+      </c>
+      <c r="G32" t="s">
+        <v>134</v>
+      </c>
+      <c r="H32" t="s">
+        <v>135</v>
+      </c>
+      <c r="I32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" t="s">
+        <v>112</v>
+      </c>
+      <c r="G33" t="s">
+        <v>112</v>
+      </c>
+      <c r="H33" t="s">
+        <v>113</v>
+      </c>
+      <c r="I33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" t="s">
+        <v>112</v>
+      </c>
+      <c r="G34" t="s">
+        <v>112</v>
+      </c>
+      <c r="H34" t="s">
+        <v>113</v>
+      </c>
+      <c r="I34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" t="s">
+        <v>134</v>
+      </c>
+      <c r="E35" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" t="s">
+        <v>134</v>
+      </c>
+      <c r="G35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H35" t="s">
+        <v>135</v>
+      </c>
+      <c r="I35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36" t="s">
+        <v>112</v>
+      </c>
+      <c r="G36" t="s">
+        <v>112</v>
+      </c>
+      <c r="H36" t="s">
+        <v>113</v>
+      </c>
+      <c r="I36" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" t="s">
+        <v>112</v>
+      </c>
+      <c r="E37" t="s">
+        <v>113</v>
+      </c>
+      <c r="F37" t="s">
+        <v>112</v>
+      </c>
+      <c r="G37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H37" t="s">
+        <v>113</v>
+      </c>
+      <c r="I37" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" t="s">
+        <v>135</v>
+      </c>
+      <c r="F38" t="s">
+        <v>134</v>
+      </c>
+      <c r="G38" t="s">
+        <v>134</v>
+      </c>
+      <c r="H38" t="s">
+        <v>135</v>
+      </c>
+      <c r="I38" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>167</v>
+      </c>
+      <c r="C39" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" t="s">
+        <v>112</v>
+      </c>
+      <c r="E39" t="s">
+        <v>113</v>
+      </c>
+      <c r="F39" t="s">
+        <v>112</v>
+      </c>
+      <c r="G39" t="s">
+        <v>112</v>
+      </c>
+      <c r="H39" t="s">
+        <v>113</v>
+      </c>
+      <c r="I39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" t="s">
+        <v>112</v>
+      </c>
+      <c r="E40" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" t="s">
+        <v>112</v>
+      </c>
+      <c r="G40" t="s">
+        <v>112</v>
+      </c>
+      <c r="H40" t="s">
+        <v>113</v>
+      </c>
+      <c r="I40" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>169</v>
+      </c>
+      <c r="C41" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" t="s">
+        <v>134</v>
+      </c>
+      <c r="E41" t="s">
+        <v>135</v>
+      </c>
+      <c r="F41" t="s">
+        <v>134</v>
+      </c>
+      <c r="G41" t="s">
+        <v>134</v>
+      </c>
+      <c r="H41" t="s">
+        <v>135</v>
+      </c>
+      <c r="I41" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>170</v>
+      </c>
+      <c r="C42" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" t="s">
+        <v>112</v>
+      </c>
+      <c r="E42" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" t="s">
+        <v>112</v>
+      </c>
+      <c r="G42" t="s">
+        <v>112</v>
+      </c>
+      <c r="H42" t="s">
+        <v>113</v>
+      </c>
+      <c r="I42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>171</v>
+      </c>
+      <c r="C43" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" t="s">
+        <v>113</v>
+      </c>
+      <c r="F43" t="s">
+        <v>112</v>
+      </c>
+      <c r="G43" t="s">
+        <v>112</v>
+      </c>
+      <c r="H43" t="s">
+        <v>113</v>
+      </c>
+      <c r="I43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" t="s">
+        <v>135</v>
+      </c>
+      <c r="F44" t="s">
+        <v>134</v>
+      </c>
+      <c r="G44" t="s">
+        <v>134</v>
+      </c>
+      <c r="H44" t="s">
+        <v>135</v>
+      </c>
+      <c r="I44" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>173</v>
+      </c>
+      <c r="C45" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" t="s">
+        <v>112</v>
+      </c>
+      <c r="E45" t="s">
+        <v>113</v>
+      </c>
+      <c r="F45" t="s">
+        <v>112</v>
+      </c>
+      <c r="G45" t="s">
+        <v>112</v>
+      </c>
+      <c r="H45" t="s">
+        <v>113</v>
+      </c>
+      <c r="I45" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>174</v>
+      </c>
+      <c r="C46" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" t="s">
+        <v>112</v>
+      </c>
+      <c r="E46" t="s">
+        <v>113</v>
+      </c>
+      <c r="F46" t="s">
+        <v>112</v>
+      </c>
+      <c r="G46" t="s">
+        <v>112</v>
+      </c>
+      <c r="H46" t="s">
+        <v>113</v>
+      </c>
+      <c r="I46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" t="s">
+        <v>134</v>
+      </c>
+      <c r="E47" t="s">
+        <v>135</v>
+      </c>
+      <c r="F47" t="s">
+        <v>134</v>
+      </c>
+      <c r="G47" t="s">
+        <v>134</v>
+      </c>
+      <c r="H47" t="s">
+        <v>135</v>
+      </c>
+      <c r="I47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" t="s">
+        <v>112</v>
+      </c>
+      <c r="E48" t="s">
+        <v>113</v>
+      </c>
+      <c r="F48" t="s">
+        <v>112</v>
+      </c>
+      <c r="G48" t="s">
+        <v>112</v>
+      </c>
+      <c r="H48" t="s">
+        <v>113</v>
+      </c>
+      <c r="I48" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49" t="s">
+        <v>111</v>
+      </c>
+      <c r="D49" t="s">
+        <v>112</v>
+      </c>
+      <c r="E49" t="s">
+        <v>113</v>
+      </c>
+      <c r="F49" t="s">
+        <v>112</v>
+      </c>
+      <c r="G49" t="s">
+        <v>112</v>
+      </c>
+      <c r="H49" t="s">
+        <v>113</v>
+      </c>
+      <c r="I49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>178</v>
+      </c>
+      <c r="C50" t="s">
+        <v>111</v>
+      </c>
+      <c r="D50" t="s">
+        <v>134</v>
+      </c>
+      <c r="E50" t="s">
+        <v>135</v>
+      </c>
+      <c r="F50" t="s">
+        <v>134</v>
+      </c>
+      <c r="G50" t="s">
+        <v>134</v>
+      </c>
+      <c r="H50" t="s">
+        <v>135</v>
+      </c>
+      <c r="I50" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>179</v>
+      </c>
+      <c r="C51" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" t="s">
+        <v>112</v>
+      </c>
+      <c r="E51" t="s">
+        <v>113</v>
+      </c>
+      <c r="F51" t="s">
+        <v>112</v>
+      </c>
+      <c r="G51" t="s">
+        <v>112</v>
+      </c>
+      <c r="H51" t="s">
+        <v>113</v>
+      </c>
+      <c r="I51" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>180</v>
+      </c>
+      <c r="C52" t="s">
+        <v>111</v>
+      </c>
+      <c r="D52" t="s">
+        <v>112</v>
+      </c>
+      <c r="E52" t="s">
+        <v>113</v>
+      </c>
+      <c r="F52" t="s">
+        <v>112</v>
+      </c>
+      <c r="G52" t="s">
+        <v>112</v>
+      </c>
+      <c r="H52" t="s">
+        <v>113</v>
+      </c>
+      <c r="I52" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>181</v>
+      </c>
+      <c r="C53" t="s">
+        <v>111</v>
+      </c>
+      <c r="D53" t="s">
+        <v>134</v>
+      </c>
+      <c r="E53" t="s">
+        <v>135</v>
+      </c>
+      <c r="F53" t="s">
+        <v>134</v>
+      </c>
+      <c r="G53" t="s">
+        <v>134</v>
+      </c>
+      <c r="H53" t="s">
+        <v>135</v>
+      </c>
+      <c r="I53" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>182</v>
+      </c>
+      <c r="C54" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" t="s">
+        <v>112</v>
+      </c>
+      <c r="E54" t="s">
+        <v>113</v>
+      </c>
+      <c r="F54" t="s">
+        <v>112</v>
+      </c>
+      <c r="G54" t="s">
+        <v>112</v>
+      </c>
+      <c r="H54" t="s">
+        <v>113</v>
+      </c>
+      <c r="I54" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>183</v>
+      </c>
+      <c r="C55" t="s">
+        <v>111</v>
+      </c>
+      <c r="D55" t="s">
+        <v>112</v>
+      </c>
+      <c r="E55" t="s">
+        <v>113</v>
+      </c>
+      <c r="F55" t="s">
+        <v>112</v>
+      </c>
+      <c r="G55" t="s">
+        <v>112</v>
+      </c>
+      <c r="H55" t="s">
+        <v>113</v>
+      </c>
+      <c r="I55" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>184</v>
+      </c>
+      <c r="C56" t="s">
+        <v>111</v>
+      </c>
+      <c r="D56" t="s">
+        <v>112</v>
+      </c>
+      <c r="E56" t="s">
+        <v>113</v>
+      </c>
+      <c r="F56" t="s">
+        <v>112</v>
+      </c>
+      <c r="G56" t="s">
+        <v>112</v>
+      </c>
+      <c r="H56" t="s">
+        <v>113</v>
+      </c>
+      <c r="I56" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>185</v>
+      </c>
+      <c r="C57" t="s">
+        <v>111</v>
+      </c>
+      <c r="D57" t="s">
+        <v>112</v>
+      </c>
+      <c r="E57" t="s">
+        <v>113</v>
+      </c>
+      <c r="F57" t="s">
+        <v>112</v>
+      </c>
+      <c r="G57" t="s">
+        <v>112</v>
+      </c>
+      <c r="H57" t="s">
+        <v>113</v>
+      </c>
+      <c r="I57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>186</v>
+      </c>
+      <c r="C58" t="s">
+        <v>111</v>
+      </c>
+      <c r="D58" t="s">
+        <v>112</v>
+      </c>
+      <c r="E58" t="s">
+        <v>113</v>
+      </c>
+      <c r="F58" t="s">
+        <v>112</v>
+      </c>
+      <c r="G58" t="s">
+        <v>112</v>
+      </c>
+      <c r="H58" t="s">
+        <v>113</v>
+      </c>
+      <c r="I58" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>187</v>
+      </c>
+      <c r="C59" t="s">
+        <v>111</v>
+      </c>
+      <c r="D59" t="s">
+        <v>112</v>
+      </c>
+      <c r="E59" t="s">
+        <v>113</v>
+      </c>
+      <c r="F59" t="s">
+        <v>112</v>
+      </c>
+      <c r="G59" t="s">
+        <v>112</v>
+      </c>
+      <c r="H59" t="s">
+        <v>113</v>
+      </c>
+      <c r="I59" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>188</v>
+      </c>
+      <c r="C60" t="s">
+        <v>111</v>
+      </c>
+      <c r="D60" t="s">
+        <v>112</v>
+      </c>
+      <c r="E60" t="s">
+        <v>113</v>
+      </c>
+      <c r="F60" t="s">
+        <v>112</v>
+      </c>
+      <c r="G60" t="s">
+        <v>112</v>
+      </c>
+      <c r="H60" t="s">
+        <v>113</v>
+      </c>
+      <c r="I60" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>189</v>
+      </c>
+      <c r="C61" t="s">
+        <v>111</v>
+      </c>
+      <c r="D61" t="s">
+        <v>112</v>
+      </c>
+      <c r="E61" t="s">
+        <v>113</v>
+      </c>
+      <c r="F61" t="s">
+        <v>112</v>
+      </c>
+      <c r="G61" t="s">
+        <v>112</v>
+      </c>
+      <c r="H61" t="s">
+        <v>113</v>
+      </c>
+      <c r="I61" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>190</v>
+      </c>
+      <c r="C62" t="s">
+        <v>111</v>
+      </c>
+      <c r="D62" t="s">
+        <v>112</v>
+      </c>
+      <c r="E62" t="s">
+        <v>113</v>
+      </c>
+      <c r="F62" t="s">
+        <v>112</v>
+      </c>
+      <c r="G62" t="s">
+        <v>112</v>
+      </c>
+      <c r="H62" t="s">
+        <v>113</v>
+      </c>
+      <c r="I62" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>191</v>
+      </c>
+      <c r="C63" t="s">
+        <v>111</v>
+      </c>
+      <c r="D63" t="s">
+        <v>112</v>
+      </c>
+      <c r="E63" t="s">
+        <v>113</v>
+      </c>
+      <c r="F63" t="s">
+        <v>112</v>
+      </c>
+      <c r="G63" t="s">
+        <v>112</v>
+      </c>
+      <c r="H63" t="s">
+        <v>113</v>
+      </c>
+      <c r="I63" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" t="s">
+        <v>111</v>
+      </c>
+      <c r="D64" t="s">
+        <v>112</v>
+      </c>
+      <c r="E64" t="s">
+        <v>113</v>
+      </c>
+      <c r="F64" t="s">
+        <v>112</v>
+      </c>
+      <c r="G64" t="s">
+        <v>112</v>
+      </c>
+      <c r="H64" t="s">
+        <v>113</v>
+      </c>
+      <c r="I64" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>193</v>
+      </c>
+      <c r="C65" t="s">
+        <v>111</v>
+      </c>
+      <c r="D65" t="s">
+        <v>112</v>
+      </c>
+      <c r="E65" t="s">
+        <v>113</v>
+      </c>
+      <c r="F65" t="s">
+        <v>112</v>
+      </c>
+      <c r="G65" t="s">
+        <v>112</v>
+      </c>
+      <c r="H65" t="s">
+        <v>113</v>
+      </c>
+      <c r="I65" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>194</v>
+      </c>
+      <c r="C66" t="s">
+        <v>111</v>
+      </c>
+      <c r="D66" t="s">
+        <v>112</v>
+      </c>
+      <c r="E66" t="s">
+        <v>113</v>
+      </c>
+      <c r="F66" t="s">
+        <v>112</v>
+      </c>
+      <c r="G66" t="s">
+        <v>112</v>
+      </c>
+      <c r="H66" t="s">
+        <v>113</v>
+      </c>
+      <c r="I66" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>195</v>
+      </c>
+      <c r="C67" t="s">
+        <v>111</v>
+      </c>
+      <c r="D67" t="s">
+        <v>112</v>
+      </c>
+      <c r="E67" t="s">
+        <v>113</v>
+      </c>
+      <c r="F67" t="s">
+        <v>112</v>
+      </c>
+      <c r="G67" t="s">
+        <v>112</v>
+      </c>
+      <c r="H67" t="s">
+        <v>113</v>
+      </c>
+      <c r="I67" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>196</v>
+      </c>
+      <c r="C68" t="s">
+        <v>111</v>
+      </c>
+      <c r="D68" t="s">
+        <v>112</v>
+      </c>
+      <c r="E68" t="s">
+        <v>113</v>
+      </c>
+      <c r="F68" t="s">
+        <v>112</v>
+      </c>
+      <c r="G68" t="s">
+        <v>112</v>
+      </c>
+      <c r="H68" t="s">
+        <v>113</v>
+      </c>
+      <c r="I68" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>197</v>
+      </c>
+      <c r="C69" t="s">
+        <v>111</v>
+      </c>
+      <c r="D69" t="s">
+        <v>112</v>
+      </c>
+      <c r="E69" t="s">
+        <v>113</v>
+      </c>
+      <c r="F69" t="s">
+        <v>112</v>
+      </c>
+      <c r="G69" t="s">
+        <v>112</v>
+      </c>
+      <c r="H69" t="s">
+        <v>113</v>
+      </c>
+      <c r="I69" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>198</v>
+      </c>
+      <c r="C70" t="s">
+        <v>111</v>
+      </c>
+      <c r="D70" t="s">
+        <v>112</v>
+      </c>
+      <c r="E70" t="s">
+        <v>113</v>
+      </c>
+      <c r="F70" t="s">
+        <v>112</v>
+      </c>
+      <c r="G70" t="s">
+        <v>112</v>
+      </c>
+      <c r="H70" t="s">
+        <v>113</v>
+      </c>
+      <c r="I70" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>199</v>
+      </c>
+      <c r="C71" t="s">
+        <v>111</v>
+      </c>
+      <c r="D71" t="s">
+        <v>112</v>
+      </c>
+      <c r="E71" t="s">
+        <v>113</v>
+      </c>
+      <c r="F71" t="s">
+        <v>112</v>
+      </c>
+      <c r="G71" t="s">
+        <v>112</v>
+      </c>
+      <c r="H71" t="s">
+        <v>113</v>
+      </c>
+      <c r="I71" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>200</v>
+      </c>
+      <c r="C72" t="s">
+        <v>111</v>
+      </c>
+      <c r="D72" t="s">
+        <v>112</v>
+      </c>
+      <c r="E72" t="s">
+        <v>113</v>
+      </c>
+      <c r="F72" t="s">
+        <v>112</v>
+      </c>
+      <c r="G72" t="s">
+        <v>112</v>
+      </c>
+      <c r="H72" t="s">
+        <v>113</v>
+      </c>
+      <c r="I72" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>201</v>
+      </c>
+      <c r="C73" t="s">
+        <v>111</v>
+      </c>
+      <c r="D73" t="s">
+        <v>112</v>
+      </c>
+      <c r="E73" t="s">
+        <v>113</v>
+      </c>
+      <c r="F73" t="s">
+        <v>112</v>
+      </c>
+      <c r="G73" t="s">
+        <v>112</v>
+      </c>
+      <c r="H73" t="s">
+        <v>113</v>
+      </c>
+      <c r="I73" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>202</v>
+      </c>
+      <c r="C74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D74" t="s">
+        <v>112</v>
+      </c>
+      <c r="E74" t="s">
+        <v>113</v>
+      </c>
+      <c r="F74" t="s">
+        <v>112</v>
+      </c>
+      <c r="G74" t="s">
+        <v>112</v>
+      </c>
+      <c r="H74" t="s">
+        <v>113</v>
+      </c>
+      <c r="I74" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>203</v>
+      </c>
+      <c r="C75" t="s">
+        <v>111</v>
+      </c>
+      <c r="D75" t="s">
+        <v>112</v>
+      </c>
+      <c r="E75" t="s">
+        <v>113</v>
+      </c>
+      <c r="F75" t="s">
+        <v>112</v>
+      </c>
+      <c r="G75" t="s">
+        <v>112</v>
+      </c>
+      <c r="H75" t="s">
+        <v>113</v>
+      </c>
+      <c r="I75" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>204</v>
+      </c>
+      <c r="C76" t="s">
+        <v>111</v>
+      </c>
+      <c r="D76" t="s">
+        <v>112</v>
+      </c>
+      <c r="E76" t="s">
+        <v>113</v>
+      </c>
+      <c r="F76" t="s">
+        <v>112</v>
+      </c>
+      <c r="G76" t="s">
+        <v>112</v>
+      </c>
+      <c r="H76" t="s">
+        <v>113</v>
+      </c>
+      <c r="I76" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>205</v>
+      </c>
+      <c r="C77" t="s">
+        <v>111</v>
+      </c>
+      <c r="D77" t="s">
+        <v>112</v>
+      </c>
+      <c r="E77" t="s">
+        <v>113</v>
+      </c>
+      <c r="F77" t="s">
+        <v>112</v>
+      </c>
+      <c r="G77" t="s">
+        <v>112</v>
+      </c>
+      <c r="H77" t="s">
+        <v>113</v>
+      </c>
+      <c r="I77" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>206</v>
+      </c>
+      <c r="C78" t="s">
+        <v>111</v>
+      </c>
+      <c r="D78" t="s">
+        <v>112</v>
+      </c>
+      <c r="E78" t="s">
+        <v>113</v>
+      </c>
+      <c r="F78" t="s">
+        <v>112</v>
+      </c>
+      <c r="G78" t="s">
+        <v>112</v>
+      </c>
+      <c r="H78" t="s">
+        <v>113</v>
+      </c>
+      <c r="I78" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>207</v>
+      </c>
+      <c r="C79" t="s">
+        <v>111</v>
+      </c>
+      <c r="D79" t="s">
+        <v>112</v>
+      </c>
+      <c r="E79" t="s">
+        <v>113</v>
+      </c>
+      <c r="F79" t="s">
+        <v>112</v>
+      </c>
+      <c r="G79" t="s">
+        <v>112</v>
+      </c>
+      <c r="H79" t="s">
+        <v>113</v>
+      </c>
+      <c r="I79" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>208</v>
+      </c>
+      <c r="C80" t="s">
+        <v>111</v>
+      </c>
+      <c r="D80" t="s">
+        <v>112</v>
+      </c>
+      <c r="E80" t="s">
+        <v>113</v>
+      </c>
+      <c r="F80" t="s">
+        <v>112</v>
+      </c>
+      <c r="G80" t="s">
+        <v>112</v>
+      </c>
+      <c r="H80" t="s">
+        <v>113</v>
+      </c>
+      <c r="I80" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>209</v>
+      </c>
+      <c r="C81" t="s">
+        <v>111</v>
+      </c>
+      <c r="D81" t="s">
+        <v>112</v>
+      </c>
+      <c r="E81" t="s">
+        <v>113</v>
+      </c>
+      <c r="F81" t="s">
+        <v>112</v>
+      </c>
+      <c r="G81" t="s">
+        <v>112</v>
+      </c>
+      <c r="H81" t="s">
+        <v>113</v>
+      </c>
+      <c r="I81" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>210</v>
+      </c>
+      <c r="C82" t="s">
+        <v>111</v>
+      </c>
+      <c r="D82" t="s">
+        <v>112</v>
+      </c>
+      <c r="E82" t="s">
+        <v>113</v>
+      </c>
+      <c r="F82" t="s">
+        <v>112</v>
+      </c>
+      <c r="G82" t="s">
+        <v>112</v>
+      </c>
+      <c r="H82" t="s">
+        <v>113</v>
+      </c>
+      <c r="I82" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>211</v>
+      </c>
+      <c r="C83" t="s">
+        <v>111</v>
+      </c>
+      <c r="D83" t="s">
+        <v>112</v>
+      </c>
+      <c r="E83" t="s">
+        <v>113</v>
+      </c>
+      <c r="F83" t="s">
+        <v>112</v>
+      </c>
+      <c r="G83" t="s">
+        <v>112</v>
+      </c>
+      <c r="H83" t="s">
+        <v>113</v>
+      </c>
+      <c r="I83" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>212</v>
+      </c>
+      <c r="C84" t="s">
+        <v>111</v>
+      </c>
+      <c r="D84" t="s">
+        <v>112</v>
+      </c>
+      <c r="E84" t="s">
+        <v>113</v>
+      </c>
+      <c r="F84" t="s">
+        <v>112</v>
+      </c>
+      <c r="G84" t="s">
+        <v>112</v>
+      </c>
+      <c r="H84" t="s">
+        <v>113</v>
+      </c>
+      <c r="I84" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>213</v>
+      </c>
+      <c r="C85" t="s">
+        <v>111</v>
+      </c>
+      <c r="D85" t="s">
+        <v>112</v>
+      </c>
+      <c r="E85" t="s">
+        <v>113</v>
+      </c>
+      <c r="F85" t="s">
+        <v>112</v>
+      </c>
+      <c r="G85" t="s">
+        <v>112</v>
+      </c>
+      <c r="H85" t="s">
+        <v>113</v>
+      </c>
+      <c r="I85" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>214</v>
+      </c>
+      <c r="C86" t="s">
+        <v>111</v>
+      </c>
+      <c r="D86" t="s">
+        <v>112</v>
+      </c>
+      <c r="E86" t="s">
+        <v>113</v>
+      </c>
+      <c r="F86" t="s">
+        <v>112</v>
+      </c>
+      <c r="G86" t="s">
+        <v>112</v>
+      </c>
+      <c r="H86" t="s">
+        <v>113</v>
+      </c>
+      <c r="I86" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>215</v>
+      </c>
+      <c r="C87" t="s">
+        <v>111</v>
+      </c>
+      <c r="D87" t="s">
+        <v>112</v>
+      </c>
+      <c r="E87" t="s">
+        <v>113</v>
+      </c>
+      <c r="F87" t="s">
+        <v>112</v>
+      </c>
+      <c r="G87" t="s">
+        <v>112</v>
+      </c>
+      <c r="H87" t="s">
+        <v>113</v>
+      </c>
+      <c r="I87" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>216</v>
+      </c>
+      <c r="C88" t="s">
+        <v>111</v>
+      </c>
+      <c r="D88" t="s">
+        <v>112</v>
+      </c>
+      <c r="E88" t="s">
+        <v>113</v>
+      </c>
+      <c r="F88" t="s">
+        <v>112</v>
+      </c>
+      <c r="G88" t="s">
+        <v>112</v>
+      </c>
+      <c r="H88" t="s">
+        <v>113</v>
+      </c>
+      <c r="I88" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>217</v>
+      </c>
+      <c r="C89" t="s">
+        <v>111</v>
+      </c>
+      <c r="D89" t="s">
+        <v>112</v>
+      </c>
+      <c r="E89" t="s">
+        <v>113</v>
+      </c>
+      <c r="F89" t="s">
+        <v>112</v>
+      </c>
+      <c r="G89" t="s">
+        <v>112</v>
+      </c>
+      <c r="H89" t="s">
+        <v>113</v>
+      </c>
+      <c r="I89" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>218</v>
+      </c>
+      <c r="C90" t="s">
+        <v>111</v>
+      </c>
+      <c r="D90" t="s">
+        <v>112</v>
+      </c>
+      <c r="E90" t="s">
+        <v>113</v>
+      </c>
+      <c r="F90" t="s">
+        <v>112</v>
+      </c>
+      <c r="G90" t="s">
+        <v>112</v>
+      </c>
+      <c r="H90" t="s">
+        <v>113</v>
+      </c>
+      <c r="I90" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>219</v>
+      </c>
+      <c r="C91" t="s">
+        <v>111</v>
+      </c>
+      <c r="D91" t="s">
+        <v>112</v>
+      </c>
+      <c r="E91" t="s">
+        <v>113</v>
+      </c>
+      <c r="F91" t="s">
+        <v>112</v>
+      </c>
+      <c r="G91" t="s">
+        <v>112</v>
+      </c>
+      <c r="H91" t="s">
+        <v>113</v>
+      </c>
+      <c r="I91" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>220</v>
+      </c>
+      <c r="C92" t="s">
+        <v>111</v>
+      </c>
+      <c r="D92" t="s">
+        <v>112</v>
+      </c>
+      <c r="E92" t="s">
+        <v>113</v>
+      </c>
+      <c r="F92" t="s">
+        <v>112</v>
+      </c>
+      <c r="G92" t="s">
+        <v>112</v>
+      </c>
+      <c r="H92" t="s">
+        <v>113</v>
+      </c>
+      <c r="I92" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>221</v>
+      </c>
+      <c r="C93" t="s">
+        <v>111</v>
+      </c>
+      <c r="D93" t="s">
+        <v>112</v>
+      </c>
+      <c r="E93" t="s">
+        <v>113</v>
+      </c>
+      <c r="F93" t="s">
+        <v>112</v>
+      </c>
+      <c r="G93" t="s">
+        <v>112</v>
+      </c>
+      <c r="H93" t="s">
+        <v>113</v>
+      </c>
+      <c r="I93" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>222</v>
+      </c>
+      <c r="C94" t="s">
+        <v>111</v>
+      </c>
+      <c r="D94" t="s">
+        <v>112</v>
+      </c>
+      <c r="E94" t="s">
+        <v>113</v>
+      </c>
+      <c r="F94" t="s">
+        <v>112</v>
+      </c>
+      <c r="G94" t="s">
+        <v>112</v>
+      </c>
+      <c r="H94" t="s">
+        <v>113</v>
+      </c>
+      <c r="I94" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>223</v>
+      </c>
+      <c r="C95" t="s">
+        <v>111</v>
+      </c>
+      <c r="D95" t="s">
+        <v>112</v>
+      </c>
+      <c r="E95" t="s">
+        <v>113</v>
+      </c>
+      <c r="F95" t="s">
+        <v>112</v>
+      </c>
+      <c r="G95" t="s">
+        <v>112</v>
+      </c>
+      <c r="H95" t="s">
+        <v>113</v>
+      </c>
+      <c r="I95" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>224</v>
+      </c>
+      <c r="C96" t="s">
+        <v>111</v>
+      </c>
+      <c r="D96" t="s">
+        <v>112</v>
+      </c>
+      <c r="E96" t="s">
+        <v>113</v>
+      </c>
+      <c r="F96" t="s">
+        <v>112</v>
+      </c>
+      <c r="G96" t="s">
+        <v>112</v>
+      </c>
+      <c r="H96" t="s">
+        <v>113</v>
+      </c>
+      <c r="I96" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>225</v>
+      </c>
+      <c r="C97" t="s">
+        <v>111</v>
+      </c>
+      <c r="D97" t="s">
+        <v>112</v>
+      </c>
+      <c r="E97" t="s">
+        <v>113</v>
+      </c>
+      <c r="F97" t="s">
+        <v>112</v>
+      </c>
+      <c r="G97" t="s">
+        <v>112</v>
+      </c>
+      <c r="H97" t="s">
+        <v>113</v>
+      </c>
+      <c r="I97" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>226</v>
+      </c>
+      <c r="C98" t="s">
+        <v>111</v>
+      </c>
+      <c r="D98" t="s">
+        <v>112</v>
+      </c>
+      <c r="E98" t="s">
+        <v>113</v>
+      </c>
+      <c r="F98" t="s">
+        <v>112</v>
+      </c>
+      <c r="G98" t="s">
+        <v>112</v>
+      </c>
+      <c r="H98" t="s">
+        <v>113</v>
+      </c>
+      <c r="I98" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>227</v>
+      </c>
+      <c r="C99" t="s">
+        <v>111</v>
+      </c>
+      <c r="D99" t="s">
+        <v>112</v>
+      </c>
+      <c r="E99" t="s">
+        <v>113</v>
+      </c>
+      <c r="F99" t="s">
+        <v>112</v>
+      </c>
+      <c r="G99" t="s">
+        <v>112</v>
+      </c>
+      <c r="H99" t="s">
+        <v>113</v>
+      </c>
+      <c r="I99" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>228</v>
+      </c>
+      <c r="C100" t="s">
+        <v>111</v>
+      </c>
+      <c r="D100" t="s">
+        <v>112</v>
+      </c>
+      <c r="E100" t="s">
+        <v>113</v>
+      </c>
+      <c r="F100" t="s">
+        <v>112</v>
+      </c>
+      <c r="G100" t="s">
+        <v>112</v>
+      </c>
+      <c r="H100" t="s">
+        <v>113</v>
+      </c>
+      <c r="I100" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>229</v>
+      </c>
+      <c r="C101" t="s">
+        <v>111</v>
+      </c>
+      <c r="D101" t="s">
+        <v>112</v>
+      </c>
+      <c r="E101" t="s">
+        <v>113</v>
+      </c>
+      <c r="F101" t="s">
+        <v>112</v>
+      </c>
+      <c r="G101" t="s">
+        <v>112</v>
+      </c>
+      <c r="H101" t="s">
+        <v>113</v>
+      </c>
+      <c r="I101" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>230</v>
+      </c>
+      <c r="C102" t="s">
+        <v>111</v>
+      </c>
+      <c r="D102" t="s">
+        <v>112</v>
+      </c>
+      <c r="E102" t="s">
+        <v>113</v>
+      </c>
+      <c r="F102" t="s">
+        <v>112</v>
+      </c>
+      <c r="G102" t="s">
+        <v>112</v>
+      </c>
+      <c r="H102" t="s">
+        <v>113</v>
+      </c>
+      <c r="I102" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>231</v>
+      </c>
+      <c r="C103" t="s">
+        <v>111</v>
+      </c>
+      <c r="D103" t="s">
+        <v>127</v>
+      </c>
+      <c r="E103" t="s">
+        <v>128</v>
+      </c>
+      <c r="F103" t="s">
+        <v>127</v>
+      </c>
+      <c r="G103" t="s">
+        <v>127</v>
+      </c>
+      <c r="H103" t="s">
+        <v>128</v>
+      </c>
+      <c r="I103" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>232</v>
+      </c>
+      <c r="C104" t="s">
+        <v>111</v>
+      </c>
+      <c r="D104" t="s">
+        <v>127</v>
+      </c>
+      <c r="E104" t="s">
+        <v>128</v>
+      </c>
+      <c r="F104" t="s">
+        <v>127</v>
+      </c>
+      <c r="G104" t="s">
+        <v>127</v>
+      </c>
+      <c r="H104" t="s">
+        <v>128</v>
+      </c>
+      <c r="I104" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>233</v>
+      </c>
+      <c r="C105" t="s">
+        <v>111</v>
+      </c>
+      <c r="D105" t="s">
+        <v>127</v>
+      </c>
+      <c r="E105" t="s">
+        <v>128</v>
+      </c>
+      <c r="F105" t="s">
+        <v>127</v>
+      </c>
+      <c r="G105" t="s">
+        <v>127</v>
+      </c>
+      <c r="H105" t="s">
+        <v>128</v>
+      </c>
+      <c r="I105" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C106" t="s">
+        <v>111</v>
+      </c>
+      <c r="D106" t="s">
+        <v>127</v>
+      </c>
+      <c r="E106" t="s">
+        <v>128</v>
+      </c>
+      <c r="F106" t="s">
+        <v>127</v>
+      </c>
+      <c r="G106" t="s">
+        <v>127</v>
+      </c>
+      <c r="H106" t="s">
+        <v>128</v>
+      </c>
+      <c r="I106" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{5F6B794E-D075-B04B-BA27-DA794C838EBB}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{5D252624-0B65-144A-9927-044C59A47BC1}"/>
+    <hyperlink ref="H2" r:id="rId3" xr:uid="{59C592C1-73C2-9149-AF92-3DB91477799D}"/>
+    <hyperlink ref="H9" r:id="rId4" xr:uid="{C0731768-7593-5046-9DF9-35DDE20379C1}"/>
+    <hyperlink ref="E10" r:id="rId5" xr:uid="{E8C7F695-681F-6045-8A3F-2AD8E228FE96}"/>
+    <hyperlink ref="E13" r:id="rId6" xr:uid="{5E078001-3EED-FB45-B3DC-108900346E26}"/>
+    <hyperlink ref="E5" r:id="rId7" xr:uid="{588023EE-6351-F041-9F3A-33F53360DFEF}"/>
+    <hyperlink ref="H13" r:id="rId8" xr:uid="{AD7500D2-D7B5-7A49-87A0-6DC91EC78D61}"/>
+    <hyperlink ref="H5" r:id="rId9" xr:uid="{43DD9C25-7D4A-2C49-9175-6F2088B22B61}"/>
+    <hyperlink ref="E105" r:id="rId10" xr:uid="{CE6EC8DB-EC08-814C-94AF-8E1C496F0C13}"/>
+    <hyperlink ref="E103" r:id="rId11" xr:uid="{6E754A32-4B2A-134D-8FE0-7FE3714AD5AE}"/>
+    <hyperlink ref="E104" r:id="rId12" xr:uid="{47D10694-AD99-7144-9F56-1A00BC7780BC}"/>
+    <hyperlink ref="E106" r:id="rId13" xr:uid="{BEB177E0-0D65-9249-A3DF-4A02246FBFBE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
construct target metadata using pydantic model.
</commit_message>
<xml_diff>
--- a/dataset_sample_2rows.xlsx
+++ b/dataset_sample_2rows.xlsx
@@ -8,13 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ot2661/Documents/01_dev/aed_pub/regimo/regimo/services/backend_regimo/data/LLEC_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCD2905-E186-AF44-8861-1775FA62A05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B418D36-F9DB-F246-A832-A050F3D6548A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="5900" windowWidth="30520" windowHeight="15980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12060" yWindow="5160" windowWidth="30520" windowHeight="15980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_sample_2rows_comp" sheetId="1" r:id="rId1"/>
     <sheet name="dataset_sample_2rows_meta" sheetId="2" r:id="rId2"/>
+    <sheet name="general" sheetId="6" r:id="rId3"/>
+    <sheet name="collection" sheetId="3" r:id="rId4"/>
+    <sheet name="context" sheetId="4" r:id="rId5"/>
+    <sheet name="licenses" sheetId="7" r:id="rId6"/>
+    <sheet name="linked_data" sheetId="8" r:id="rId7"/>
+    <sheet name="meta" sheetId="9" r:id="rId8"/>
+    <sheet name="provenance" sheetId="10" r:id="rId9"/>
+    <sheet name="review" sheetId="11" r:id="rId10"/>
+    <sheet name="sources" sheetId="12" r:id="rId11"/>
+    <sheet name="spatial" sheetId="13" r:id="rId12"/>
+    <sheet name="temporal" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,8 +47,22 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{CDA5DDA5-BF29-484B-9E67-07650E65A988}" keepAlive="1" name="Query - Query" description="Connection to the 'Query' query in the workbook." type="5" refreshedVersion="0" background="1">
+    <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Query;Extended Properties=&quot;&quot;" command="SELECT * FROM [Query]"/>
+  </connection>
+  <connection id="2" xr16:uid="{65FD02E7-A15A-AE4D-A729-54C65D723345}" keepAlive="1" name="Query - Query (2)" description="Connection to the 'Query (2)' query in the workbook." type="5" refreshedVersion="0" background="1">
+    <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Query (2)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Query (2)]"/>
+  </connection>
+  <connection id="3" xr16:uid="{14415025-657A-8C47-A27E-05D8AB95B730}" keepAlive="1" name="Query - Query (3)" description="Connection to the 'Query (3)' query in the workbook." type="5" refreshedVersion="0" background="1">
+    <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Query (3)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Query (3)]"/>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="268">
   <si>
     <t>t_amb</t>
   </si>
@@ -757,6 +782,90 @@
   </si>
   <si>
     <t>valueReference.path</t>
+  </si>
+  <si>
+    <t>topics</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>languages</t>
+  </si>
+  <si>
+    <t>"en-GB"</t>
+  </si>
+  <si>
+    <t>subject.name</t>
+  </si>
+  <si>
+    <t>subject.path</t>
+  </si>
+  <si>
+    <t>keywords</t>
+  </si>
+  <si>
+    <t>publicationDate</t>
+  </si>
+  <si>
+    <t>embargoPeriod.start</t>
+  </si>
+  <si>
+    <t>embargoPeriod.end</t>
+  </si>
+  <si>
+    <t>embargoPeriod.isActive</t>
+  </si>
+  <si>
+    <t>Living Lab Measurements</t>
+  </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>https://github.com/koubaa-hmc/LLEC_Data/raw/refs/heads/main/dataset_sample_2rows.xlsx</t>
+  </si>
+  <si>
+    <t>The table is a collection of measurements done in a Living Lab</t>
+  </si>
+  <si>
+    <t>http://openenergy-platform.org/ontology/oeo/OEO_00010210</t>
+  </si>
+  <si>
+    <t>energy use</t>
+  </si>
+  <si>
+    <t>http://openenergy-platform.org/ontology/oeo/OEO_00000150</t>
+  </si>
+  <si>
+    <t>http://openenergy-platform.org/ontology/oeo/OEO_00000384</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>third</t>
+  </si>
+  <si>
+    <t>fourth</t>
+  </si>
+  <si>
+    <t>Propoerty</t>
+  </si>
+  <si>
+    <t>first_or_single</t>
   </si>
 </sst>
 </file>
@@ -809,7 +918,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -819,6 +928,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1102,7 +1212,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DB3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2008,12 +2120,60 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8C9924-C26B-D644-8404-43325131289E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF507BF-54D7-BA4D-97AA-90679F613835}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC2ACAA-63F6-324C-81DA-AFBFFBD6F581}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB491E8-EBD9-C243-A5C4-BA053C8F6779}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D989DE-C4AF-CF4B-A769-6611C82EBD6C}">
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2129,6 +2289,7 @@
       <c r="D4" t="s">
         <v>120</v>
       </c>
+      <c r="E4" s="4"/>
       <c r="F4" t="s">
         <v>120</v>
       </c>
@@ -5115,4 +5276,224 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F846AC-FBFC-FA42-AB8B-D6A5014E852E}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="6" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B11" s="7">
+        <v>45685</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{C8BC289C-2E94-8A40-8F32-C6499B3E579F}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{F541954F-50FD-2145-9928-5FD1B85E7B2B}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{437B2934-4E50-BC44-9544-5F9ECA355C1A}"/>
+    <hyperlink ref="C10" r:id="rId4" xr:uid="{BBD2CEAC-0FF2-6049-A544-74439276D6B5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE67855-489F-0F49-96B0-9BABBD6DC490}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9E7B78-11CA-554C-888A-A7F69D58129D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEFE41F3-2870-8E46-9786-C10DF7867159}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E4D0C8-B442-3940-A815-42F8C658D25E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2D55EE-4790-F54C-BCFC-9261193150C3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D6034B-6506-5F46-AB99-5A3F0364E638}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>